<commit_message>
Most updated generated CEA files on 29Jan18
More Updated than the previous commit
</commit_message>
<xml_diff>
--- a/urban_design/cea_excel/age.xlsx
+++ b/urban_design/cea_excel/age.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="241">
   <si>
     <t>Name</t>
   </si>
@@ -582,6 +582,171 @@
   </si>
   <si>
     <t>B178</t>
+  </si>
+  <si>
+    <t>B179</t>
+  </si>
+  <si>
+    <t>B180</t>
+  </si>
+  <si>
+    <t>B181</t>
+  </si>
+  <si>
+    <t>B182</t>
+  </si>
+  <si>
+    <t>B183</t>
+  </si>
+  <si>
+    <t>B184</t>
+  </si>
+  <si>
+    <t>B185</t>
+  </si>
+  <si>
+    <t>B186</t>
+  </si>
+  <si>
+    <t>B187</t>
+  </si>
+  <si>
+    <t>B188</t>
+  </si>
+  <si>
+    <t>B189</t>
+  </si>
+  <si>
+    <t>B190</t>
+  </si>
+  <si>
+    <t>B191</t>
+  </si>
+  <si>
+    <t>B192</t>
+  </si>
+  <si>
+    <t>B193</t>
+  </si>
+  <si>
+    <t>B194</t>
+  </si>
+  <si>
+    <t>B195</t>
+  </si>
+  <si>
+    <t>B196</t>
+  </si>
+  <si>
+    <t>B197</t>
+  </si>
+  <si>
+    <t>B198</t>
+  </si>
+  <si>
+    <t>B199</t>
+  </si>
+  <si>
+    <t>B200</t>
+  </si>
+  <si>
+    <t>B201</t>
+  </si>
+  <si>
+    <t>B202</t>
+  </si>
+  <si>
+    <t>B203</t>
+  </si>
+  <si>
+    <t>B204</t>
+  </si>
+  <si>
+    <t>B205</t>
+  </si>
+  <si>
+    <t>B206</t>
+  </si>
+  <si>
+    <t>B207</t>
+  </si>
+  <si>
+    <t>B208</t>
+  </si>
+  <si>
+    <t>B209</t>
+  </si>
+  <si>
+    <t>B210</t>
+  </si>
+  <si>
+    <t>B211</t>
+  </si>
+  <si>
+    <t>B212</t>
+  </si>
+  <si>
+    <t>B213</t>
+  </si>
+  <si>
+    <t>B214</t>
+  </si>
+  <si>
+    <t>B215</t>
+  </si>
+  <si>
+    <t>B216</t>
+  </si>
+  <si>
+    <t>B217</t>
+  </si>
+  <si>
+    <t>B218</t>
+  </si>
+  <si>
+    <t>B219</t>
+  </si>
+  <si>
+    <t>B220</t>
+  </si>
+  <si>
+    <t>B221</t>
+  </si>
+  <si>
+    <t>B222</t>
+  </si>
+  <si>
+    <t>B223</t>
+  </si>
+  <si>
+    <t>B224</t>
+  </si>
+  <si>
+    <t>B225</t>
+  </si>
+  <si>
+    <t>B226</t>
+  </si>
+  <si>
+    <t>B227</t>
+  </si>
+  <si>
+    <t>B228</t>
+  </si>
+  <si>
+    <t>B229</t>
+  </si>
+  <si>
+    <t>B230</t>
+  </si>
+  <si>
+    <t>B231</t>
+  </si>
+  <si>
+    <t>B232</t>
+  </si>
+  <si>
+    <t>B233</t>
   </si>
 </sst>
 </file>
@@ -899,7 +1064,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H179"/>
+  <dimension ref="A1:H234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5559,6 +5724,1436 @@
         <v>0</v>
       </c>
     </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>186</v>
+      </c>
+      <c r="B180">
+        <v>2018</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="G180">
+        <v>0</v>
+      </c>
+      <c r="H180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>187</v>
+      </c>
+      <c r="B181">
+        <v>2018</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+      <c r="G181">
+        <v>0</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>188</v>
+      </c>
+      <c r="B182">
+        <v>2018</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="G182">
+        <v>0</v>
+      </c>
+      <c r="H182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>189</v>
+      </c>
+      <c r="B183">
+        <v>2018</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <v>0</v>
+      </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>190</v>
+      </c>
+      <c r="B184">
+        <v>2018</v>
+      </c>
+      <c r="C184">
+        <v>0</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184">
+        <v>0</v>
+      </c>
+      <c r="H184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>191</v>
+      </c>
+      <c r="B185">
+        <v>2018</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="H185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>192</v>
+      </c>
+      <c r="B186">
+        <v>2018</v>
+      </c>
+      <c r="C186">
+        <v>0</v>
+      </c>
+      <c r="D186">
+        <v>0</v>
+      </c>
+      <c r="E186">
+        <v>0</v>
+      </c>
+      <c r="F186">
+        <v>0</v>
+      </c>
+      <c r="G186">
+        <v>0</v>
+      </c>
+      <c r="H186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>193</v>
+      </c>
+      <c r="B187">
+        <v>2018</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="D187">
+        <v>0</v>
+      </c>
+      <c r="E187">
+        <v>0</v>
+      </c>
+      <c r="F187">
+        <v>0</v>
+      </c>
+      <c r="G187">
+        <v>0</v>
+      </c>
+      <c r="H187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>194</v>
+      </c>
+      <c r="B188">
+        <v>2018</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188">
+        <v>0</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>195</v>
+      </c>
+      <c r="B189">
+        <v>2018</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>0</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>196</v>
+      </c>
+      <c r="B190">
+        <v>2018</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="D190">
+        <v>0</v>
+      </c>
+      <c r="E190">
+        <v>0</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+      <c r="G190">
+        <v>0</v>
+      </c>
+      <c r="H190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>197</v>
+      </c>
+      <c r="B191">
+        <v>2018</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
+      </c>
+      <c r="D191">
+        <v>0</v>
+      </c>
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
+      <c r="H191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>198</v>
+      </c>
+      <c r="B192">
+        <v>2018</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>199</v>
+      </c>
+      <c r="B193">
+        <v>2018</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193">
+        <v>0</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>200</v>
+      </c>
+      <c r="B194">
+        <v>2018</v>
+      </c>
+      <c r="C194">
+        <v>0</v>
+      </c>
+      <c r="D194">
+        <v>0</v>
+      </c>
+      <c r="E194">
+        <v>0</v>
+      </c>
+      <c r="F194">
+        <v>0</v>
+      </c>
+      <c r="G194">
+        <v>0</v>
+      </c>
+      <c r="H194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>201</v>
+      </c>
+      <c r="B195">
+        <v>2018</v>
+      </c>
+      <c r="C195">
+        <v>0</v>
+      </c>
+      <c r="D195">
+        <v>0</v>
+      </c>
+      <c r="E195">
+        <v>0</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="G195">
+        <v>0</v>
+      </c>
+      <c r="H195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>202</v>
+      </c>
+      <c r="B196">
+        <v>2018</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196">
+        <v>0</v>
+      </c>
+      <c r="F196">
+        <v>0</v>
+      </c>
+      <c r="G196">
+        <v>0</v>
+      </c>
+      <c r="H196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>203</v>
+      </c>
+      <c r="B197">
+        <v>2018</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197">
+        <v>0</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+      <c r="G197">
+        <v>0</v>
+      </c>
+      <c r="H197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>204</v>
+      </c>
+      <c r="B198">
+        <v>2018</v>
+      </c>
+      <c r="C198">
+        <v>0</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198">
+        <v>0</v>
+      </c>
+      <c r="F198">
+        <v>0</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>205</v>
+      </c>
+      <c r="B199">
+        <v>2018</v>
+      </c>
+      <c r="C199">
+        <v>0</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <v>0</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+      <c r="G199">
+        <v>0</v>
+      </c>
+      <c r="H199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>206</v>
+      </c>
+      <c r="B200">
+        <v>2018</v>
+      </c>
+      <c r="C200">
+        <v>0</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>0</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+      <c r="G200">
+        <v>0</v>
+      </c>
+      <c r="H200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>207</v>
+      </c>
+      <c r="B201">
+        <v>2018</v>
+      </c>
+      <c r="C201">
+        <v>0</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="E201">
+        <v>0</v>
+      </c>
+      <c r="F201">
+        <v>0</v>
+      </c>
+      <c r="G201">
+        <v>0</v>
+      </c>
+      <c r="H201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>208</v>
+      </c>
+      <c r="B202">
+        <v>2018</v>
+      </c>
+      <c r="C202">
+        <v>0</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202">
+        <v>0</v>
+      </c>
+      <c r="F202">
+        <v>0</v>
+      </c>
+      <c r="G202">
+        <v>0</v>
+      </c>
+      <c r="H202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>209</v>
+      </c>
+      <c r="B203">
+        <v>2018</v>
+      </c>
+      <c r="C203">
+        <v>0</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="E203">
+        <v>0</v>
+      </c>
+      <c r="F203">
+        <v>0</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
+      <c r="H203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>210</v>
+      </c>
+      <c r="B204">
+        <v>2018</v>
+      </c>
+      <c r="C204">
+        <v>0</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204">
+        <v>0</v>
+      </c>
+      <c r="F204">
+        <v>0</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>211</v>
+      </c>
+      <c r="B205">
+        <v>2018</v>
+      </c>
+      <c r="C205">
+        <v>0</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205">
+        <v>0</v>
+      </c>
+      <c r="F205">
+        <v>0</v>
+      </c>
+      <c r="G205">
+        <v>0</v>
+      </c>
+      <c r="H205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>212</v>
+      </c>
+      <c r="B206">
+        <v>2018</v>
+      </c>
+      <c r="C206">
+        <v>0</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>0</v>
+      </c>
+      <c r="F206">
+        <v>0</v>
+      </c>
+      <c r="G206">
+        <v>0</v>
+      </c>
+      <c r="H206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>213</v>
+      </c>
+      <c r="B207">
+        <v>2018</v>
+      </c>
+      <c r="C207">
+        <v>0</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207">
+        <v>0</v>
+      </c>
+      <c r="F207">
+        <v>0</v>
+      </c>
+      <c r="G207">
+        <v>0</v>
+      </c>
+      <c r="H207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>214</v>
+      </c>
+      <c r="B208">
+        <v>2018</v>
+      </c>
+      <c r="C208">
+        <v>0</v>
+      </c>
+      <c r="D208">
+        <v>0</v>
+      </c>
+      <c r="E208">
+        <v>0</v>
+      </c>
+      <c r="F208">
+        <v>0</v>
+      </c>
+      <c r="G208">
+        <v>0</v>
+      </c>
+      <c r="H208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>215</v>
+      </c>
+      <c r="B209">
+        <v>2018</v>
+      </c>
+      <c r="C209">
+        <v>0</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209">
+        <v>0</v>
+      </c>
+      <c r="F209">
+        <v>0</v>
+      </c>
+      <c r="G209">
+        <v>0</v>
+      </c>
+      <c r="H209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>216</v>
+      </c>
+      <c r="B210">
+        <v>2018</v>
+      </c>
+      <c r="C210">
+        <v>0</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>0</v>
+      </c>
+      <c r="F210">
+        <v>0</v>
+      </c>
+      <c r="G210">
+        <v>0</v>
+      </c>
+      <c r="H210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>217</v>
+      </c>
+      <c r="B211">
+        <v>2018</v>
+      </c>
+      <c r="C211">
+        <v>0</v>
+      </c>
+      <c r="D211">
+        <v>0</v>
+      </c>
+      <c r="E211">
+        <v>0</v>
+      </c>
+      <c r="F211">
+        <v>0</v>
+      </c>
+      <c r="G211">
+        <v>0</v>
+      </c>
+      <c r="H211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>218</v>
+      </c>
+      <c r="B212">
+        <v>2018</v>
+      </c>
+      <c r="C212">
+        <v>0</v>
+      </c>
+      <c r="D212">
+        <v>0</v>
+      </c>
+      <c r="E212">
+        <v>0</v>
+      </c>
+      <c r="F212">
+        <v>0</v>
+      </c>
+      <c r="G212">
+        <v>0</v>
+      </c>
+      <c r="H212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>219</v>
+      </c>
+      <c r="B213">
+        <v>2018</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213">
+        <v>0</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="G213">
+        <v>0</v>
+      </c>
+      <c r="H213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>220</v>
+      </c>
+      <c r="B214">
+        <v>2018</v>
+      </c>
+      <c r="C214">
+        <v>0</v>
+      </c>
+      <c r="D214">
+        <v>0</v>
+      </c>
+      <c r="E214">
+        <v>0</v>
+      </c>
+      <c r="F214">
+        <v>0</v>
+      </c>
+      <c r="G214">
+        <v>0</v>
+      </c>
+      <c r="H214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>221</v>
+      </c>
+      <c r="B215">
+        <v>2018</v>
+      </c>
+      <c r="C215">
+        <v>0</v>
+      </c>
+      <c r="D215">
+        <v>0</v>
+      </c>
+      <c r="E215">
+        <v>0</v>
+      </c>
+      <c r="F215">
+        <v>0</v>
+      </c>
+      <c r="G215">
+        <v>0</v>
+      </c>
+      <c r="H215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>222</v>
+      </c>
+      <c r="B216">
+        <v>2018</v>
+      </c>
+      <c r="C216">
+        <v>0</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>0</v>
+      </c>
+      <c r="F216">
+        <v>0</v>
+      </c>
+      <c r="G216">
+        <v>0</v>
+      </c>
+      <c r="H216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>223</v>
+      </c>
+      <c r="B217">
+        <v>2018</v>
+      </c>
+      <c r="C217">
+        <v>0</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>0</v>
+      </c>
+      <c r="F217">
+        <v>0</v>
+      </c>
+      <c r="G217">
+        <v>0</v>
+      </c>
+      <c r="H217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>224</v>
+      </c>
+      <c r="B218">
+        <v>2018</v>
+      </c>
+      <c r="C218">
+        <v>0</v>
+      </c>
+      <c r="D218">
+        <v>0</v>
+      </c>
+      <c r="E218">
+        <v>0</v>
+      </c>
+      <c r="F218">
+        <v>0</v>
+      </c>
+      <c r="G218">
+        <v>0</v>
+      </c>
+      <c r="H218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>225</v>
+      </c>
+      <c r="B219">
+        <v>2018</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>0</v>
+      </c>
+      <c r="F219">
+        <v>0</v>
+      </c>
+      <c r="G219">
+        <v>0</v>
+      </c>
+      <c r="H219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>226</v>
+      </c>
+      <c r="B220">
+        <v>2018</v>
+      </c>
+      <c r="C220">
+        <v>0</v>
+      </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>0</v>
+      </c>
+      <c r="F220">
+        <v>0</v>
+      </c>
+      <c r="G220">
+        <v>0</v>
+      </c>
+      <c r="H220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>227</v>
+      </c>
+      <c r="B221">
+        <v>2018</v>
+      </c>
+      <c r="C221">
+        <v>0</v>
+      </c>
+      <c r="D221">
+        <v>0</v>
+      </c>
+      <c r="E221">
+        <v>0</v>
+      </c>
+      <c r="F221">
+        <v>0</v>
+      </c>
+      <c r="G221">
+        <v>0</v>
+      </c>
+      <c r="H221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>228</v>
+      </c>
+      <c r="B222">
+        <v>2018</v>
+      </c>
+      <c r="C222">
+        <v>0</v>
+      </c>
+      <c r="D222">
+        <v>0</v>
+      </c>
+      <c r="E222">
+        <v>0</v>
+      </c>
+      <c r="F222">
+        <v>0</v>
+      </c>
+      <c r="G222">
+        <v>0</v>
+      </c>
+      <c r="H222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>229</v>
+      </c>
+      <c r="B223">
+        <v>2018</v>
+      </c>
+      <c r="C223">
+        <v>0</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+      <c r="E223">
+        <v>0</v>
+      </c>
+      <c r="F223">
+        <v>0</v>
+      </c>
+      <c r="G223">
+        <v>0</v>
+      </c>
+      <c r="H223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>230</v>
+      </c>
+      <c r="B224">
+        <v>2018</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224">
+        <v>0</v>
+      </c>
+      <c r="F224">
+        <v>0</v>
+      </c>
+      <c r="G224">
+        <v>0</v>
+      </c>
+      <c r="H224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>231</v>
+      </c>
+      <c r="B225">
+        <v>2018</v>
+      </c>
+      <c r="C225">
+        <v>0</v>
+      </c>
+      <c r="D225">
+        <v>0</v>
+      </c>
+      <c r="E225">
+        <v>0</v>
+      </c>
+      <c r="F225">
+        <v>0</v>
+      </c>
+      <c r="G225">
+        <v>0</v>
+      </c>
+      <c r="H225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>232</v>
+      </c>
+      <c r="B226">
+        <v>2018</v>
+      </c>
+      <c r="C226">
+        <v>0</v>
+      </c>
+      <c r="D226">
+        <v>0</v>
+      </c>
+      <c r="E226">
+        <v>0</v>
+      </c>
+      <c r="F226">
+        <v>0</v>
+      </c>
+      <c r="G226">
+        <v>0</v>
+      </c>
+      <c r="H226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>233</v>
+      </c>
+      <c r="B227">
+        <v>2018</v>
+      </c>
+      <c r="C227">
+        <v>0</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
+      <c r="E227">
+        <v>0</v>
+      </c>
+      <c r="F227">
+        <v>0</v>
+      </c>
+      <c r="G227">
+        <v>0</v>
+      </c>
+      <c r="H227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>234</v>
+      </c>
+      <c r="B228">
+        <v>2018</v>
+      </c>
+      <c r="C228">
+        <v>0</v>
+      </c>
+      <c r="D228">
+        <v>0</v>
+      </c>
+      <c r="E228">
+        <v>0</v>
+      </c>
+      <c r="F228">
+        <v>0</v>
+      </c>
+      <c r="G228">
+        <v>0</v>
+      </c>
+      <c r="H228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>235</v>
+      </c>
+      <c r="B229">
+        <v>2018</v>
+      </c>
+      <c r="C229">
+        <v>0</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+      <c r="E229">
+        <v>0</v>
+      </c>
+      <c r="F229">
+        <v>0</v>
+      </c>
+      <c r="G229">
+        <v>0</v>
+      </c>
+      <c r="H229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>236</v>
+      </c>
+      <c r="B230">
+        <v>2018</v>
+      </c>
+      <c r="C230">
+        <v>0</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>0</v>
+      </c>
+      <c r="F230">
+        <v>0</v>
+      </c>
+      <c r="G230">
+        <v>0</v>
+      </c>
+      <c r="H230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>237</v>
+      </c>
+      <c r="B231">
+        <v>2018</v>
+      </c>
+      <c r="C231">
+        <v>0</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+      <c r="E231">
+        <v>0</v>
+      </c>
+      <c r="F231">
+        <v>0</v>
+      </c>
+      <c r="G231">
+        <v>0</v>
+      </c>
+      <c r="H231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>238</v>
+      </c>
+      <c r="B232">
+        <v>2018</v>
+      </c>
+      <c r="C232">
+        <v>0</v>
+      </c>
+      <c r="D232">
+        <v>0</v>
+      </c>
+      <c r="E232">
+        <v>0</v>
+      </c>
+      <c r="F232">
+        <v>0</v>
+      </c>
+      <c r="G232">
+        <v>0</v>
+      </c>
+      <c r="H232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>239</v>
+      </c>
+      <c r="B233">
+        <v>2018</v>
+      </c>
+      <c r="C233">
+        <v>0</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>0</v>
+      </c>
+      <c r="F233">
+        <v>0</v>
+      </c>
+      <c r="G233">
+        <v>0</v>
+      </c>
+      <c r="H233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>240</v>
+      </c>
+      <c r="B234">
+        <v>2018</v>
+      </c>
+      <c r="C234">
+        <v>0</v>
+      </c>
+      <c r="D234">
+        <v>0</v>
+      </c>
+      <c r="E234">
+        <v>0</v>
+      </c>
+      <c r="F234">
+        <v>0</v>
+      </c>
+      <c r="G234">
+        <v>0</v>
+      </c>
+      <c r="H234">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>